<commit_message>
Modified Certification page, added manage listings and description, added change password files
</commit_message>
<xml_diff>
--- a/AdvancedTask2.xlsx
+++ b/AdvancedTask2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Hema\IndustryConnect\Internship\AdvancedTaskPart2\AdvancedTaskMarsPart2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C89E67BC-1E7D-4D1B-B19D-318EC918EB8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E299E639-A404-441E-9CE3-5E5DC5F1372C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="165">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -169,22 +169,6 @@
     <t>TC_202</t>
   </si>
   <si>
-    <t xml:space="preserve">Verify if user able to edit education </t>
-  </si>
-  <si>
-    <t>1. University of Canterbury
-2. Selected New Zealand
-3. Selected MBA
-4. Master of Applied Computing
-5. Selected 2022</t>
-  </si>
-  <si>
-    <t>Education updated successfully</t>
-  </si>
-  <si>
-    <t>Education has been updated</t>
-  </si>
-  <si>
     <t>TC_203</t>
   </si>
   <si>
@@ -219,9 +203,6 @@
     <t>Please enter all the fields</t>
   </si>
   <si>
-    <t>TC_205</t>
-  </si>
-  <si>
     <t xml:space="preserve">Verify if user able to cancel while editing </t>
   </si>
   <si>
@@ -601,6 +582,15 @@
   </si>
   <si>
     <t>TC_102</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify if user able to add existing education </t>
+  </si>
+  <si>
+    <t>Education not saved</t>
+  </si>
+  <si>
+    <t>Education already existing</t>
   </si>
 </sst>
 </file>
@@ -952,8 +942,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13:K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1039,13 +1029,13 @@
     </row>
     <row r="6" spans="1:11" ht="180" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>21</v>
@@ -1075,13 +1065,13 @@
     <row r="7" spans="1:11" ht="180" x14ac:dyDescent="0.25">
       <c r="B7" s="4"/>
       <c r="C7" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>26</v>
@@ -1090,24 +1080,24 @@
         <v>22</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="255" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C8" t="s">
         <v>27</v>
@@ -1168,7 +1158,7 @@
         <v>40</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>41</v>
+        <v>162</v>
       </c>
       <c r="E10" t="s">
         <v>36</v>
@@ -1180,24 +1170,24 @@
         <v>31</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>43</v>
+        <v>163</v>
       </c>
       <c r="J10" s="4" t="s">
         <v>25</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>44</v>
+        <v>164</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="255" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E11" t="s">
         <v>36</v>
@@ -1210,24 +1200,24 @@
       </c>
       <c r="H11" s="4"/>
       <c r="I11" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="J11" s="4" t="s">
         <v>25</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="255" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E12" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>30</v>
@@ -1236,56 +1226,36 @@
         <v>31</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="J12" s="4" t="s">
         <v>25</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="255" x14ac:dyDescent="0.25">
-      <c r="C13" t="s">
-        <v>55</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="E13" t="s">
-        <v>36</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="I13" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="J13" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="K13" s="4" t="s">
-        <v>58</v>
-      </c>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
     </row>
     <row r="14" spans="1:11" ht="255" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E14" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>30</v>
@@ -1294,27 +1264,27 @@
         <v>31</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="255" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E15" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>30</v>
@@ -1323,27 +1293,27 @@
         <v>31</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="J15" s="4" t="s">
         <v>25</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="255" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E16" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>30</v>
@@ -1352,16 +1322,16 @@
         <v>31</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1392,7 +1362,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>15</v>
@@ -1427,16 +1397,16 @@
     </row>
     <row r="2" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C2" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="E2" t="s">
         <v>29</v>
@@ -1445,7 +1415,7 @@
         <v>30</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>32</v>
@@ -1459,10 +1429,10 @@
     </row>
     <row r="3" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E3" t="s">
         <v>36</v>
@@ -1471,27 +1441,27 @@
         <v>30</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="J3" s="4" t="s">
         <v>25</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="E4" t="s">
         <v>36</v>
@@ -1500,27 +1470,27 @@
         <v>30</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="J4" s="4" t="s">
         <v>25</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="E5" t="s">
         <v>36</v>
@@ -1529,54 +1499,54 @@
         <v>30</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="H5" s="4"/>
       <c r="I5" s="4" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="J5" s="4" t="s">
         <v>25</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="E6" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>30</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="J6" s="4" t="s">
         <v>25</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="E7" t="s">
         <v>36</v>
@@ -1585,141 +1555,141 @@
         <v>30</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="J7" s="4" t="s">
         <v>25</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E8" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>30</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E9" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>30</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="J9" s="4" t="s">
         <v>25</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E10" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>30</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C11" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E11" t="s">
         <v>36</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="J11" s="4" t="s">
         <v>25</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1750,7 +1720,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>15</v>
@@ -1786,122 +1756,122 @@
     </row>
     <row r="2" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C2" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E2" t="s">
         <v>36</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="J2" t="s">
         <v>25</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="135" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="E3" t="s">
         <v>36</v>
       </c>
       <c r="F3" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>114</v>
-      </c>
       <c r="H3" s="4" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="J3" t="s">
         <v>25</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="120" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="E4" t="s">
         <v>36</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="H4" s="4"/>
       <c r="I4" s="4" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="J4" t="s">
         <v>25</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="C5" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="E5" t="s">
         <v>36</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="J5" s="4" t="s">
         <v>25</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -1925,7 +1895,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>15</v>
@@ -1960,87 +1930,87 @@
     </row>
     <row r="2" spans="1:11" ht="180" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="C2" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="E2" t="s">
         <v>36</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>25</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="180" x14ac:dyDescent="0.25">
       <c r="B3" s="4"/>
       <c r="C3" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="E3" t="s">
         <v>36</v>
       </c>
       <c r="F3" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>137</v>
-      </c>
       <c r="I3" s="4" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="J3" s="4" t="s">
         <v>25</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="225" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="E4" t="s">
         <v>36</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="J4" s="4" t="s">
         <v>25</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>

</xml_diff>